<commit_message>
update week 4 timesheet
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/week4/HuyNguyen_timesheet_wk4.xlsx
+++ b/Documentation/TimeSheets/week4/HuyNguyen_timesheet_wk4.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>Informal meeting 2nd</t>
+  </si>
+  <si>
+    <t>SRS draft preperation</t>
+  </si>
+  <si>
+    <t>Ant tool research for build file</t>
   </si>
 </sst>
 </file>
@@ -454,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -548,7 +554,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" ref="G8:G10" si="0">(F8-E8)</f>
+        <f t="shared" ref="G8:G11" si="0">(F8-E8)</f>
         <v>1.388888888888884E-2</v>
       </c>
     </row>
@@ -589,18 +595,40 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
+        <v>42967</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="5">
+        <f>(F11-E11)</f>
+        <v>0.16666666666666669</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3">
+        <v>42967</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="G12" s="5">
+        <f>(F12-E12)</f>
+        <v>6.25E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="2"/>
@@ -660,7 +688,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="6">
         <f>SUM(G7:G19)</f>
-        <v>0.2847222222222221</v>
+        <v>0.51388888888888884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>